<commit_message>
[Issue 3509] Relaxed the non-blank TC name rule enforced by workbook parser
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/missing-headers.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/missing-headers.xlsx
@@ -28,9 +28,6 @@
     <t>PROJECT_NAME</t>
   </si>
   <si>
-    <t>TC_PATH</t>
-  </si>
-  <si>
     <t>TC_NUM</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>TC_#_CALLED_BY</t>
+  </si>
+  <si>
+    <t>TC_NAME</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,69 +594,69 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -683,7 +683,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -710,7 +710,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -737,7 +737,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -764,7 +764,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -791,7 +791,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -818,7 +818,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -845,7 +845,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -897,7 +897,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>

</xml_diff>